<commit_message>
metadata from July ctenidia RNA isolation
</commit_message>
<xml_diff>
--- a/Data/RNA-DNA-Isolation/Sample-inventory-June2019.xlsx
+++ b/Data/RNA-DNA-Isolation/Sample-inventory-June2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laura/Documents/roberts-lab/O.lurida_Stress/Data/RNA-DNA-Isolation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA64260-7FAC-5349-9C48-EB9FD5FF564F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D416FE-8721-414C-A5F1-D155361CFC04}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="460" windowWidth="27000" windowHeight="17540" xr2:uid="{0808AB85-DD2A-B240-A6C3-759B97F851D8}"/>
+    <workbookView xWindow="15700" yWindow="460" windowWidth="13100" windowHeight="17540" activeTab="2" xr2:uid="{0808AB85-DD2A-B240-A6C3-759B97F851D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Larval samples" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Deployment samples'!$A$1:$J$616</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Larval samples'!$A$3:$H$3</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1715" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1995" uniqueCount="198">
   <si>
     <t xml:space="preserve">Frozen larvae, sampled day of release, pooled by spawn bucket. </t>
   </si>
@@ -579,16 +579,58 @@
     <t>Eelgrass</t>
   </si>
   <si>
-    <t>Do just Dabob Bay and Fidalgo Bay, both whole-body and gill samples, all in same site (port gamble, eelgrass)</t>
-  </si>
-  <si>
-    <t>&gt; 38 samples</t>
-  </si>
-  <si>
     <t xml:space="preserve">Deployment samples </t>
   </si>
   <si>
     <t>Larval samples</t>
+  </si>
+  <si>
+    <t>All Fidalgo &amp; Dabob Bay Cohorts</t>
+  </si>
+  <si>
+    <t>Just Eelgrass</t>
+  </si>
+  <si>
+    <t>Just Whole Body, eelgrass</t>
+  </si>
+  <si>
+    <t>Just Whole Body, eelgrass &amp; bare</t>
+  </si>
+  <si>
+    <t>Samples</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Pouch</t>
+  </si>
+  <si>
+    <t>I think pouch 25 actually was 24</t>
+  </si>
+  <si>
+    <t>TISSUE TYPE</t>
+  </si>
+  <si>
+    <t>% Survival</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>1 lane of sequencing = 70 samples</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>ambient</t>
+  </si>
+  <si>
+    <t>Skokomish</t>
+  </si>
+  <si>
+    <t>Case Inlet</t>
   </si>
 </sst>
 </file>
@@ -600,7 +642,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -647,6 +689,23 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -710,11 +769,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -793,10 +853,56 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1110,8 +1216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF4CFDE5-1E37-584B-A2C8-7BB39BD0FF4A}">
   <dimension ref="A1:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="J76" sqref="J76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3658,7 +3764,7 @@
   <dimension ref="A1:J616"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+      <selection activeCell="I625" sqref="I625"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3708,6 +3814,9 @@
       <c r="D2">
         <v>141</v>
       </c>
+      <c r="E2" t="s">
+        <v>154</v>
+      </c>
       <c r="F2">
         <v>20.64</v>
       </c>
@@ -3737,6 +3846,9 @@
       <c r="D3">
         <v>141</v>
       </c>
+      <c r="E3" t="s">
+        <v>154</v>
+      </c>
       <c r="F3">
         <v>26.4</v>
       </c>
@@ -3766,6 +3878,9 @@
       <c r="D4">
         <v>141</v>
       </c>
+      <c r="E4" t="s">
+        <v>154</v>
+      </c>
       <c r="F4">
         <v>25.52</v>
       </c>
@@ -3795,6 +3910,9 @@
       <c r="D5">
         <v>141</v>
       </c>
+      <c r="E5" t="s">
+        <v>154</v>
+      </c>
       <c r="F5">
         <v>20.89</v>
       </c>
@@ -3853,6 +3971,9 @@
       <c r="D7">
         <v>31</v>
       </c>
+      <c r="E7" t="s">
+        <v>151</v>
+      </c>
       <c r="F7">
         <v>25.48</v>
       </c>
@@ -3879,6 +4000,9 @@
       <c r="D8">
         <v>31</v>
       </c>
+      <c r="E8" t="s">
+        <v>151</v>
+      </c>
       <c r="F8">
         <v>29.63</v>
       </c>
@@ -4028,7 +4152,7 @@
         <v>0.51666666666666672</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="25">
         <v>43349</v>
       </c>
@@ -4041,6 +4165,9 @@
       <c r="D14">
         <v>47</v>
       </c>
+      <c r="E14" t="s">
+        <v>153</v>
+      </c>
       <c r="F14">
         <v>25.08</v>
       </c>
@@ -4057,7 +4184,7 @@
         <v>0.51666666666666672</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="25">
         <v>43349</v>
       </c>
@@ -4070,6 +4197,9 @@
       <c r="D15">
         <v>47</v>
       </c>
+      <c r="E15" t="s">
+        <v>153</v>
+      </c>
       <c r="F15">
         <v>23.14</v>
       </c>
@@ -4086,7 +4216,7 @@
         <v>0.51666666666666672</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="25">
         <v>43349</v>
       </c>
@@ -4099,6 +4229,9 @@
       <c r="D16">
         <v>47</v>
       </c>
+      <c r="E16" t="s">
+        <v>153</v>
+      </c>
       <c r="F16">
         <v>23.7</v>
       </c>
@@ -4115,7 +4248,7 @@
         <v>0.51666666666666672</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="25">
         <v>43349</v>
       </c>
@@ -4128,6 +4261,9 @@
       <c r="D17">
         <v>47</v>
       </c>
+      <c r="E17" t="s">
+        <v>153</v>
+      </c>
       <c r="F17">
         <v>24.24</v>
       </c>
@@ -4144,7 +4280,7 @@
         <v>0.51666666666666672</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="25">
         <v>43349</v>
       </c>
@@ -4157,6 +4293,9 @@
       <c r="D18">
         <v>47</v>
       </c>
+      <c r="E18" t="s">
+        <v>153</v>
+      </c>
       <c r="F18">
         <v>20.77</v>
       </c>
@@ -4173,7 +4312,7 @@
         <v>0.51666666666666672</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="25">
         <v>43349</v>
       </c>
@@ -4185,6 +4324,9 @@
       </c>
       <c r="D19">
         <v>86</v>
+      </c>
+      <c r="E19" t="s">
+        <v>149</v>
       </c>
       <c r="F19">
         <v>13.57</v>
@@ -4210,10 +4352,13 @@
         <v>157</v>
       </c>
       <c r="C20" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="D20">
         <v>110</v>
+      </c>
+      <c r="E20" t="s">
+        <v>155</v>
       </c>
       <c r="F20">
         <v>25.34</v>
@@ -4239,10 +4384,13 @@
         <v>157</v>
       </c>
       <c r="C21" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="D21">
         <v>110</v>
+      </c>
+      <c r="E21" t="s">
+        <v>155</v>
       </c>
       <c r="F21">
         <v>22.39</v>
@@ -4268,10 +4416,13 @@
         <v>157</v>
       </c>
       <c r="C22" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="D22">
         <v>110</v>
+      </c>
+      <c r="E22" t="s">
+        <v>155</v>
       </c>
       <c r="F22">
         <v>22.96</v>
@@ -4297,11 +4448,14 @@
         <v>157</v>
       </c>
       <c r="C23" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="D23">
         <v>110</v>
       </c>
+      <c r="E23" t="s">
+        <v>155</v>
+      </c>
       <c r="F23">
         <v>25.97</v>
       </c>
@@ -4318,7 +4472,7 @@
         <v>5.2083333333333336E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="25">
         <v>43349</v>
       </c>
@@ -4330,6 +4484,9 @@
       </c>
       <c r="D24">
         <v>64</v>
+      </c>
+      <c r="E24" t="s">
+        <v>152</v>
       </c>
       <c r="F24">
         <v>16.18</v>
@@ -4737,6 +4894,9 @@
       <c r="D38">
         <v>116</v>
       </c>
+      <c r="E38" t="s">
+        <v>155</v>
+      </c>
       <c r="F38">
         <v>29.98</v>
       </c>
@@ -4766,6 +4926,9 @@
       <c r="D39">
         <v>116</v>
       </c>
+      <c r="E39" t="s">
+        <v>155</v>
+      </c>
       <c r="F39">
         <v>29.39</v>
       </c>
@@ -4795,6 +4958,9 @@
       <c r="D40">
         <v>116</v>
       </c>
+      <c r="E40" t="s">
+        <v>155</v>
+      </c>
       <c r="F40">
         <v>23.57</v>
       </c>
@@ -4824,6 +4990,9 @@
       <c r="D41">
         <v>33</v>
       </c>
+      <c r="E41" t="s">
+        <v>151</v>
+      </c>
       <c r="F41">
         <v>23.55</v>
       </c>
@@ -4853,6 +5022,9 @@
       <c r="D42">
         <v>33</v>
       </c>
+      <c r="E42" t="s">
+        <v>151</v>
+      </c>
       <c r="F42">
         <v>21.02</v>
       </c>
@@ -4882,6 +5054,9 @@
       <c r="D43">
         <v>33</v>
       </c>
+      <c r="E43" t="s">
+        <v>151</v>
+      </c>
       <c r="F43">
         <v>29.05</v>
       </c>
@@ -4911,6 +5086,9 @@
       <c r="D44">
         <v>33</v>
       </c>
+      <c r="E44" t="s">
+        <v>151</v>
+      </c>
       <c r="F44">
         <v>24.23</v>
       </c>
@@ -4940,6 +5118,9 @@
       <c r="D45">
         <v>33</v>
       </c>
+      <c r="E45" t="s">
+        <v>151</v>
+      </c>
       <c r="F45">
         <v>25.88</v>
       </c>
@@ -4969,6 +5150,9 @@
       <c r="D46">
         <v>43</v>
       </c>
+      <c r="E46" t="s">
+        <v>153</v>
+      </c>
       <c r="F46">
         <v>18.079999999999998</v>
       </c>
@@ -5439,6 +5623,9 @@
       <c r="D62">
         <v>31</v>
       </c>
+      <c r="E62" t="s">
+        <v>151</v>
+      </c>
       <c r="F62">
         <v>23.44</v>
       </c>
@@ -5465,6 +5652,9 @@
       <c r="D63">
         <v>31</v>
       </c>
+      <c r="E63" t="s">
+        <v>151</v>
+      </c>
       <c r="F63">
         <v>23.45</v>
       </c>
@@ -5647,6 +5837,9 @@
       <c r="D70">
         <v>31</v>
       </c>
+      <c r="E70" t="s">
+        <v>151</v>
+      </c>
       <c r="F70">
         <v>28.54</v>
       </c>
@@ -5660,7 +5853,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="25">
         <v>43349</v>
       </c>
@@ -5673,6 +5866,9 @@
       <c r="D71">
         <v>160</v>
       </c>
+      <c r="E71" t="s">
+        <v>150</v>
+      </c>
       <c r="F71">
         <v>24.33</v>
       </c>
@@ -5686,7 +5882,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="25">
         <v>43349</v>
       </c>
@@ -5699,6 +5895,9 @@
       <c r="D72">
         <v>160</v>
       </c>
+      <c r="E72" t="s">
+        <v>150</v>
+      </c>
       <c r="F72">
         <v>28.37</v>
       </c>
@@ -5712,7 +5911,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="25">
         <v>43349</v>
       </c>
@@ -5725,6 +5924,9 @@
       <c r="D73">
         <v>160</v>
       </c>
+      <c r="E73" t="s">
+        <v>150</v>
+      </c>
       <c r="F73">
         <v>25.61</v>
       </c>
@@ -5738,7 +5940,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="25">
         <v>43349</v>
       </c>
@@ -5751,6 +5953,9 @@
       <c r="D74">
         <v>158</v>
       </c>
+      <c r="E74" t="s">
+        <v>154</v>
+      </c>
       <c r="F74">
         <v>22.35</v>
       </c>
@@ -5764,7 +5969,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="25">
         <v>43349</v>
       </c>
@@ -5777,6 +5982,9 @@
       <c r="D75">
         <v>158</v>
       </c>
+      <c r="E75" t="s">
+        <v>154</v>
+      </c>
       <c r="F75">
         <v>22.31</v>
       </c>
@@ -5790,7 +5998,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="25">
         <v>43349</v>
       </c>
@@ -5803,6 +6011,9 @@
       <c r="D76">
         <v>158</v>
       </c>
+      <c r="E76" t="s">
+        <v>154</v>
+      </c>
       <c r="F76">
         <v>26.01</v>
       </c>
@@ -5816,7 +6027,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="25">
         <v>43349</v>
       </c>
@@ -5829,6 +6040,9 @@
       <c r="D77">
         <v>158</v>
       </c>
+      <c r="E77" t="s">
+        <v>154</v>
+      </c>
       <c r="F77">
         <v>19.28</v>
       </c>
@@ -5842,7 +6056,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="25">
         <v>43349</v>
       </c>
@@ -5855,6 +6069,9 @@
       <c r="D78">
         <v>158</v>
       </c>
+      <c r="E78" t="s">
+        <v>154</v>
+      </c>
       <c r="F78">
         <v>27.81</v>
       </c>
@@ -5868,7 +6085,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="25">
         <v>43349</v>
       </c>
@@ -5881,6 +6098,9 @@
       <c r="D79">
         <v>35</v>
       </c>
+      <c r="E79" t="s">
+        <v>151</v>
+      </c>
       <c r="F79">
         <v>14.34</v>
       </c>
@@ -5894,7 +6114,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="25">
         <v>43349</v>
       </c>
@@ -5907,6 +6127,9 @@
       <c r="D80">
         <v>35</v>
       </c>
+      <c r="E80" t="s">
+        <v>151</v>
+      </c>
       <c r="F80">
         <v>20.96</v>
       </c>
@@ -5920,7 +6143,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="25">
         <v>43349</v>
       </c>
@@ -5933,6 +6156,9 @@
       <c r="D81">
         <v>35</v>
       </c>
+      <c r="E81" t="s">
+        <v>151</v>
+      </c>
       <c r="F81">
         <v>27.05</v>
       </c>
@@ -5946,7 +6172,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="25">
         <v>43349</v>
       </c>
@@ -5959,6 +6185,9 @@
       <c r="D82">
         <v>35</v>
       </c>
+      <c r="E82" t="s">
+        <v>151</v>
+      </c>
       <c r="F82">
         <v>25.41</v>
       </c>
@@ -5972,7 +6201,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="25">
         <v>43349</v>
       </c>
@@ -5984,6 +6213,9 @@
       </c>
       <c r="D83">
         <v>35</v>
+      </c>
+      <c r="E83" t="s">
+        <v>151</v>
       </c>
       <c r="F83">
         <v>20.59</v>
@@ -6874,6 +7106,9 @@
       <c r="D115">
         <v>159</v>
       </c>
+      <c r="E115" t="s">
+        <v>150</v>
+      </c>
       <c r="F115">
         <v>23.04</v>
       </c>
@@ -6903,6 +7138,9 @@
       <c r="D116">
         <v>159</v>
       </c>
+      <c r="E116" t="s">
+        <v>150</v>
+      </c>
       <c r="F116">
         <v>24.5</v>
       </c>
@@ -6932,6 +7170,9 @@
       <c r="D117">
         <v>159</v>
       </c>
+      <c r="E117" t="s">
+        <v>150</v>
+      </c>
       <c r="F117">
         <v>26.46</v>
       </c>
@@ -6960,6 +7201,9 @@
       </c>
       <c r="D118">
         <v>159</v>
+      </c>
+      <c r="E118" t="s">
+        <v>150</v>
       </c>
       <c r="F118">
         <v>25.26</v>
@@ -13063,6 +13307,11 @@
     <filterColumn colId="1">
       <filters>
         <filter val="FB"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="E"/>
       </filters>
     </filterColumn>
     <filterColumn colId="7">
@@ -13077,29 +13326,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56BFE4F2-3B9A-D04A-8ED1-C8E3E4D4A170}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="F41" workbookViewId="0">
+      <selection activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
     <col min="3" max="3" width="12.83203125" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" customWidth="1"/>
+    <col min="11" max="11" width="14.1640625" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="30" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="30" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G1" s="30" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="33" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="33" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
         <v>114</v>
       </c>
@@ -13122,16 +13374,22 @@
         <v>171</v>
       </c>
       <c r="J2" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="K2" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="L2" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="L2" s="29" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M2" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="N2" s="33" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>117</v>
       </c>
@@ -13144,26 +13402,32 @@
       <c r="D3" s="24">
         <v>4</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="I3" s="27">
-        <v>5</v>
-      </c>
-      <c r="J3" s="27" t="s">
+      <c r="I3" s="43">
+        <v>3</v>
+      </c>
+      <c r="J3" s="43">
+        <v>89</v>
+      </c>
+      <c r="K3" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="L3" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="L3" s="27" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M3" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="N3" s="46">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>117</v>
       </c>
@@ -13176,26 +13440,32 @@
       <c r="D4" s="24">
         <v>2</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="I4" s="27">
-        <v>4</v>
-      </c>
-      <c r="J4" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="K4" s="27" t="s">
-        <v>178</v>
-      </c>
-      <c r="L4" s="27" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I4" s="43">
+        <v>3</v>
+      </c>
+      <c r="J4" s="43">
+        <v>25</v>
+      </c>
+      <c r="K4" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="L4" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="M4" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="N4" s="46">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>117</v>
       </c>
@@ -13208,26 +13478,32 @@
       <c r="D5" s="24">
         <v>0</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="I5" s="28">
-        <v>5</v>
-      </c>
-      <c r="J5" s="28" t="s">
+      <c r="I5" s="44">
+        <v>3</v>
+      </c>
+      <c r="J5" s="44">
+        <v>61</v>
+      </c>
+      <c r="K5" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="K5" s="28" t="s">
-        <v>176</v>
-      </c>
-      <c r="L5" s="28" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L5" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="M5" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="N5" s="47">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>117</v>
       </c>
@@ -13240,26 +13516,32 @@
       <c r="D6" s="24">
         <v>3</v>
       </c>
-      <c r="G6" s="28" t="s">
+      <c r="G6" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="H6" s="28" t="s">
+      <c r="H6" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="I6" s="28">
-        <v>5</v>
-      </c>
-      <c r="J6" s="28" t="s">
+      <c r="I6" s="44">
+        <v>3</v>
+      </c>
+      <c r="J6" s="44">
+        <v>94</v>
+      </c>
+      <c r="K6" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="K6" s="28" t="s">
-        <v>178</v>
-      </c>
-      <c r="L6" s="28" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L6" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="M6" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="N6" s="47">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
         <v>118</v>
       </c>
@@ -13272,26 +13554,35 @@
       <c r="D7" s="24">
         <v>5</v>
       </c>
-      <c r="G7" t="s">
+      <c r="F7" s="45" t="s">
+        <v>189</v>
+      </c>
+      <c r="G7" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="H7" t="s">
-        <v>175</v>
-      </c>
-      <c r="I7">
-        <v>5</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="H7" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="I7" s="44">
+        <v>3</v>
+      </c>
+      <c r="J7" s="44">
+        <v>3</v>
+      </c>
+      <c r="K7" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="K7" t="s">
-        <v>176</v>
-      </c>
-      <c r="L7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L7" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="M7" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="N7" s="47">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
         <v>118</v>
       </c>
@@ -13304,26 +13595,32 @@
       <c r="D8" s="24">
         <v>3</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="H8" t="s">
-        <v>175</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="H8" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="I8" s="44">
+        <v>3</v>
+      </c>
+      <c r="J8" s="44">
+        <v>32</v>
+      </c>
+      <c r="K8" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="K8" t="s">
-        <v>178</v>
-      </c>
-      <c r="L8" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L8" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="M8" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="N8" s="47">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>118</v>
       </c>
@@ -13336,26 +13633,32 @@
       <c r="D9" s="24">
         <v>2</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="H9" s="28" t="s">
-        <v>179</v>
-      </c>
-      <c r="I9" s="28">
+      <c r="H9" s="35" t="s">
+        <v>175</v>
+      </c>
+      <c r="I9" s="39">
         <v>5</v>
       </c>
-      <c r="J9" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="K9" s="28" t="s">
+      <c r="J9" s="39">
+        <v>89</v>
+      </c>
+      <c r="K9" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="L9" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="L9" s="28" t="s">
+      <c r="M9" s="35" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N9" s="48">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
         <v>118</v>
       </c>
@@ -13368,26 +13671,32 @@
       <c r="D10" s="24">
         <v>7</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="H10" s="28" t="s">
-        <v>179</v>
-      </c>
-      <c r="I10" s="28">
-        <v>5</v>
-      </c>
-      <c r="J10" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="K10" s="28" t="s">
+      <c r="H10" s="35" t="s">
+        <v>175</v>
+      </c>
+      <c r="I10" s="39">
+        <v>4</v>
+      </c>
+      <c r="J10" s="39">
+        <v>63</v>
+      </c>
+      <c r="K10" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="L10" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="L10" s="28" t="s">
+      <c r="M10" s="35" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N10" s="48">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
         <v>115</v>
       </c>
@@ -13400,90 +13709,108 @@
       <c r="D11" s="24">
         <v>13</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="35" t="s">
         <v>175</v>
       </c>
-      <c r="I11">
-        <v>4</v>
-      </c>
-      <c r="J11" t="s">
-        <v>115</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="I11" s="39">
+        <v>5</v>
+      </c>
+      <c r="J11" s="39">
+        <v>25</v>
+      </c>
+      <c r="K11" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="L11" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" s="35" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N11" s="48">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>115</v>
       </c>
       <c r="B12" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="50">
         <v>8</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="50">
         <v>0</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="H12" t="s">
-        <v>179</v>
-      </c>
-      <c r="I12">
-        <v>5</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="H12" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="I12" s="41">
+        <v>4</v>
+      </c>
+      <c r="J12" s="41">
+        <v>152</v>
+      </c>
+      <c r="K12" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="K12" t="s">
-        <v>178</v>
-      </c>
-      <c r="L12" t="s">
+      <c r="L12" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="M12" s="28" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N12" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
         <v>115</v>
       </c>
       <c r="B13" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="C13" s="24">
+      <c r="C13" s="50">
         <v>7</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="50">
         <v>0</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="H13" t="s">
-        <v>175</v>
-      </c>
-      <c r="I13">
-        <v>3</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="H13" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="I13" s="40">
+        <v>5</v>
+      </c>
+      <c r="J13" s="40">
+        <v>94</v>
+      </c>
+      <c r="K13" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="L13" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M13" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="N13" s="49">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
         <v>115</v>
       </c>
@@ -13496,26 +13823,32 @@
       <c r="D14" s="24">
         <v>10</v>
       </c>
-      <c r="G14" s="28" t="s">
+      <c r="G14" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="H14" s="28" t="s">
+      <c r="H14" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="I14" s="28">
-        <v>3</v>
-      </c>
-      <c r="J14" s="28" t="s">
+      <c r="I14" s="40">
+        <v>5</v>
+      </c>
+      <c r="J14" s="40">
+        <v>61</v>
+      </c>
+      <c r="K14" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="K14" s="28" t="s">
+      <c r="L14" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="L14" s="28" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M14" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="N14" s="49">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>116</v>
       </c>
@@ -13528,26 +13861,32 @@
       <c r="D15" s="24">
         <v>3</v>
       </c>
-      <c r="G15" s="28" t="s">
+      <c r="G15" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="H15" s="28" t="s">
+      <c r="H15" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="I15" s="28">
-        <v>3</v>
-      </c>
-      <c r="J15" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="K15" s="28" t="s">
+      <c r="I15" s="40">
+        <v>5</v>
+      </c>
+      <c r="J15" s="40">
+        <v>32</v>
+      </c>
+      <c r="K15" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="L15" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="L15" s="28" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M15" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="N15" s="49">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
         <v>116</v>
       </c>
@@ -13560,26 +13899,32 @@
       <c r="D16" s="24">
         <v>3</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="H16" t="s">
-        <v>175</v>
-      </c>
-      <c r="I16">
+      <c r="H16" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="I16" s="40">
+        <v>5</v>
+      </c>
+      <c r="J16" s="40">
         <v>3</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="K16" t="s">
-        <v>176</v>
-      </c>
-      <c r="L16" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L16" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="M16" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="N16" s="49">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
         <v>116</v>
       </c>
@@ -13592,26 +13937,32 @@
       <c r="D17" s="24">
         <v>4</v>
       </c>
-      <c r="G17" s="28" t="s">
+      <c r="G17" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="H17" s="28" t="s">
+      <c r="H17" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="I17" s="28">
-        <v>3</v>
-      </c>
-      <c r="J17" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="K17" s="28" t="s">
+      <c r="I17" s="42">
+        <v>5</v>
+      </c>
+      <c r="J17" s="42">
+        <v>111</v>
+      </c>
+      <c r="K17" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="L17" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="L17" s="28" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M17" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="N17" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
         <v>116</v>
       </c>
@@ -13624,36 +13975,1272 @@
       <c r="D18" s="24">
         <v>5</v>
       </c>
-      <c r="G18" s="28" t="s">
-        <v>174</v>
-      </c>
-      <c r="H18" s="28" t="s">
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H19" s="38" t="s">
+        <v>186</v>
+      </c>
+      <c r="I19" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="J19" s="38"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B20" s="51" t="s">
+        <v>192</v>
+      </c>
+      <c r="C20" s="29">
+        <f>SUM(C3:C18)-8</f>
+        <v>75</v>
+      </c>
+      <c r="H20" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="I20" s="29">
+        <f>SUM(I12:I17,I8:I9,I3:I7)</f>
+        <v>52</v>
+      </c>
+      <c r="J20" s="29"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H21" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="I21" s="29">
+        <f>SUM(I16:I17,I13:I14,I8:I9,I5:I6)</f>
+        <v>34</v>
+      </c>
+      <c r="J21" s="29"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="52" t="s">
+        <v>193</v>
+      </c>
+      <c r="H22" s="37" t="s">
+        <v>184</v>
+      </c>
+      <c r="I22" s="29">
+        <f>SUM(I5:I6,I8:I9)</f>
+        <v>14</v>
+      </c>
+      <c r="J22" s="29"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H23" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="I23" s="29">
+        <f>SUM(I3:I7,I8:I9)</f>
+        <v>23</v>
+      </c>
+      <c r="J23" s="29"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G25" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="H25" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I25">
+        <v>3</v>
+      </c>
+      <c r="J25">
+        <v>47</v>
+      </c>
+      <c r="K25" t="s">
+        <v>118</v>
+      </c>
+      <c r="L25" t="s">
+        <v>195</v>
+      </c>
+      <c r="M25" t="s">
+        <v>143</v>
+      </c>
+      <c r="N25" s="56">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G26" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="H26" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I26">
+        <v>3</v>
+      </c>
+      <c r="J26">
+        <v>35</v>
+      </c>
+      <c r="K26" t="s">
+        <v>118</v>
+      </c>
+      <c r="L26" t="s">
+        <v>194</v>
+      </c>
+      <c r="M26" t="s">
+        <v>143</v>
+      </c>
+      <c r="N26" s="56">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G27" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="H27" s="54" t="s">
         <v>179</v>
       </c>
-      <c r="I18" s="28">
+      <c r="I27">
         <v>3</v>
       </c>
-      <c r="J18" s="28" t="s">
+      <c r="J27">
+        <v>31</v>
+      </c>
+      <c r="K27" t="s">
         <v>118</v>
       </c>
-      <c r="K18" s="28" t="s">
-        <v>176</v>
-      </c>
-      <c r="L18" s="28" t="s">
+      <c r="L27" t="s">
+        <v>194</v>
+      </c>
+      <c r="M27" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G21" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G22" t="s">
-        <v>181</v>
-      </c>
+      <c r="N27" s="56">
+        <v>0.93300000000000005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G28" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="H28" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>86</v>
+      </c>
+      <c r="K28" t="s">
+        <v>117</v>
+      </c>
+      <c r="L28" t="s">
+        <v>194</v>
+      </c>
+      <c r="M28" t="s">
+        <v>177</v>
+      </c>
+      <c r="N28" s="56">
+        <v>6.6600000000000006E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G29" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="H29" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>64</v>
+      </c>
+      <c r="K29" t="s">
+        <v>117</v>
+      </c>
+      <c r="L29" t="s">
+        <v>195</v>
+      </c>
+      <c r="M29" t="s">
+        <v>177</v>
+      </c>
+      <c r="N29" s="56">
+        <v>6.6600000000000006E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G30" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="H30" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I30">
+        <v>5</v>
+      </c>
+      <c r="J30">
+        <v>47</v>
+      </c>
+      <c r="K30" t="s">
+        <v>118</v>
+      </c>
+      <c r="L30" t="s">
+        <v>195</v>
+      </c>
+      <c r="M30" t="s">
+        <v>177</v>
+      </c>
+      <c r="N30" s="56">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G31" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="H31" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I31">
+        <v>5</v>
+      </c>
+      <c r="J31">
+        <v>35</v>
+      </c>
+      <c r="K31" t="s">
+        <v>118</v>
+      </c>
+      <c r="L31" t="s">
+        <v>194</v>
+      </c>
+      <c r="M31" t="s">
+        <v>177</v>
+      </c>
+      <c r="N31" s="56">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G32" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="H32" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I32">
+        <v>5</v>
+      </c>
+      <c r="J32">
+        <v>158</v>
+      </c>
+      <c r="K32" t="s">
+        <v>115</v>
+      </c>
+      <c r="L32" t="s">
+        <v>194</v>
+      </c>
+      <c r="M32" t="s">
+        <v>177</v>
+      </c>
+      <c r="N32" s="56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G33" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="H33" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I33">
+        <v>3</v>
+      </c>
+      <c r="J33">
+        <v>160</v>
+      </c>
+      <c r="K33" t="s">
+        <v>116</v>
+      </c>
+      <c r="L33" t="s">
+        <v>195</v>
+      </c>
+      <c r="M33" t="s">
+        <v>177</v>
+      </c>
+      <c r="N33" s="56">
+        <v>0.214</v>
+      </c>
+    </row>
+    <row r="34" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G34" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="H34" s="54" t="s">
+        <v>179</v>
+      </c>
+      <c r="I34">
+        <v>5</v>
+      </c>
+      <c r="J34">
+        <v>31</v>
+      </c>
+      <c r="K34" t="s">
+        <v>118</v>
+      </c>
+      <c r="L34" t="s">
+        <v>194</v>
+      </c>
+      <c r="M34" t="s">
+        <v>177</v>
+      </c>
+      <c r="N34" s="56">
+        <v>0.93300000000000005</v>
+      </c>
+    </row>
+    <row r="35" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G35" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="H35" s="54" t="s">
+        <v>179</v>
+      </c>
+      <c r="I35">
+        <v>4</v>
+      </c>
+      <c r="J35">
+        <v>141</v>
+      </c>
+      <c r="K35" t="s">
+        <v>115</v>
+      </c>
+      <c r="L35" t="s">
+        <v>194</v>
+      </c>
+      <c r="M35" t="s">
+        <v>177</v>
+      </c>
+      <c r="N35" s="56">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="36" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G36" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="H36" s="54" t="s">
+        <v>179</v>
+      </c>
+      <c r="I36">
+        <v>4</v>
+      </c>
+      <c r="J36">
+        <v>110</v>
+      </c>
+      <c r="K36" t="s">
+        <v>115</v>
+      </c>
+      <c r="L36" t="s">
+        <v>195</v>
+      </c>
+      <c r="M36" t="s">
+        <v>177</v>
+      </c>
+      <c r="N36" s="56">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="38" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G38" t="s">
+        <v>196</v>
+      </c>
+      <c r="H38" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>67</v>
+      </c>
+      <c r="K38" t="s">
+        <v>117</v>
+      </c>
+      <c r="L38" t="s">
+        <v>195</v>
+      </c>
+      <c r="M38" t="s">
+        <v>143</v>
+      </c>
+      <c r="N38" s="56">
+        <v>0.46600000000000003</v>
+      </c>
+    </row>
+    <row r="39" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G39" t="s">
+        <v>196</v>
+      </c>
+      <c r="H39" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="J39">
+        <v>45</v>
+      </c>
+      <c r="K39" t="s">
+        <v>118</v>
+      </c>
+      <c r="L39" t="s">
+        <v>195</v>
+      </c>
+      <c r="M39" t="s">
+        <v>143</v>
+      </c>
+      <c r="N39" s="56">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="40" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G40" t="s">
+        <v>196</v>
+      </c>
+      <c r="H40" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I40">
+        <v>3</v>
+      </c>
+      <c r="J40">
+        <v>36</v>
+      </c>
+      <c r="K40" t="s">
+        <v>118</v>
+      </c>
+      <c r="L40" t="s">
+        <v>194</v>
+      </c>
+      <c r="M40" t="s">
+        <v>143</v>
+      </c>
+      <c r="N40" s="56">
+        <v>0.66700000000000004</v>
+      </c>
+    </row>
+    <row r="41" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G41" t="s">
+        <v>196</v>
+      </c>
+      <c r="H41" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I41">
+        <v>3</v>
+      </c>
+      <c r="J41">
+        <v>34</v>
+      </c>
+      <c r="K41" t="s">
+        <v>118</v>
+      </c>
+      <c r="L41" t="s">
+        <v>194</v>
+      </c>
+      <c r="M41" t="s">
+        <v>143</v>
+      </c>
+      <c r="N41" s="56">
+        <v>0.66700000000000004</v>
+      </c>
+    </row>
+    <row r="42" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G42" t="s">
+        <v>196</v>
+      </c>
+      <c r="H42" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I42">
+        <v>2</v>
+      </c>
+      <c r="J42">
+        <v>166</v>
+      </c>
+      <c r="K42" t="s">
+        <v>116</v>
+      </c>
+      <c r="L42" t="s">
+        <v>195</v>
+      </c>
+      <c r="M42" t="s">
+        <v>143</v>
+      </c>
+      <c r="N42" s="56">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="43" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G43" t="s">
+        <v>196</v>
+      </c>
+      <c r="H43" s="54" t="s">
+        <v>179</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+      <c r="J43">
+        <v>70</v>
+      </c>
+      <c r="K43" t="s">
+        <v>117</v>
+      </c>
+      <c r="L43" t="s">
+        <v>195</v>
+      </c>
+      <c r="M43" t="s">
+        <v>143</v>
+      </c>
+      <c r="N43" s="56">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="44" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G44" t="s">
+        <v>196</v>
+      </c>
+      <c r="H44" s="54" t="s">
+        <v>179</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="J44">
+        <v>4</v>
+      </c>
+      <c r="K44" t="s">
+        <v>118</v>
+      </c>
+      <c r="L44" t="s">
+        <v>195</v>
+      </c>
+      <c r="M44" t="s">
+        <v>143</v>
+      </c>
+      <c r="N44" s="56">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="45" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G45" t="s">
+        <v>196</v>
+      </c>
+      <c r="H45" s="54" t="s">
+        <v>179</v>
+      </c>
+      <c r="I45">
+        <v>3</v>
+      </c>
+      <c r="J45">
+        <v>21</v>
+      </c>
+      <c r="K45" t="s">
+        <v>118</v>
+      </c>
+      <c r="L45" t="s">
+        <v>194</v>
+      </c>
+      <c r="M45" t="s">
+        <v>143</v>
+      </c>
+      <c r="N45" s="56">
+        <v>0.86660000000000004</v>
+      </c>
+    </row>
+    <row r="46" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G46" t="s">
+        <v>196</v>
+      </c>
+      <c r="H46" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I46">
+        <v>4</v>
+      </c>
+      <c r="J46">
+        <v>91</v>
+      </c>
+      <c r="K46" t="s">
+        <v>117</v>
+      </c>
+      <c r="L46" t="s">
+        <v>194</v>
+      </c>
+      <c r="M46" t="s">
+        <v>177</v>
+      </c>
+      <c r="N46" s="56">
+        <v>0.2666</v>
+      </c>
+    </row>
+    <row r="47" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G47" t="s">
+        <v>196</v>
+      </c>
+      <c r="H47" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I47">
+        <v>5</v>
+      </c>
+      <c r="J47">
+        <v>67</v>
+      </c>
+      <c r="K47" t="s">
+        <v>117</v>
+      </c>
+      <c r="L47" t="s">
+        <v>195</v>
+      </c>
+      <c r="M47" t="s">
+        <v>177</v>
+      </c>
+      <c r="N47" s="56">
+        <v>0.46600000000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G48" t="s">
+        <v>196</v>
+      </c>
+      <c r="H48" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I48">
+        <v>5</v>
+      </c>
+      <c r="J48">
+        <v>45</v>
+      </c>
+      <c r="K48" t="s">
+        <v>118</v>
+      </c>
+      <c r="L48" t="s">
+        <v>195</v>
+      </c>
+      <c r="M48" t="s">
+        <v>177</v>
+      </c>
+      <c r="N48" s="56">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="49" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G49" t="s">
+        <v>196</v>
+      </c>
+      <c r="H49" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I49">
+        <v>5</v>
+      </c>
+      <c r="J49">
+        <v>36</v>
+      </c>
+      <c r="K49" t="s">
+        <v>118</v>
+      </c>
+      <c r="L49" t="s">
+        <v>194</v>
+      </c>
+      <c r="M49" t="s">
+        <v>177</v>
+      </c>
+      <c r="N49" s="56">
+        <v>0.66700000000000004</v>
+      </c>
+    </row>
+    <row r="50" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G50" t="s">
+        <v>196</v>
+      </c>
+      <c r="H50" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I50">
+        <v>5</v>
+      </c>
+      <c r="J50">
+        <v>34</v>
+      </c>
+      <c r="K50" t="s">
+        <v>118</v>
+      </c>
+      <c r="L50" t="s">
+        <v>194</v>
+      </c>
+      <c r="M50" t="s">
+        <v>177</v>
+      </c>
+      <c r="N50" s="56">
+        <v>0.66700000000000004</v>
+      </c>
+    </row>
+    <row r="51" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G51" t="s">
+        <v>196</v>
+      </c>
+      <c r="H51" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I51">
+        <v>5</v>
+      </c>
+      <c r="J51">
+        <v>166</v>
+      </c>
+      <c r="K51" t="s">
+        <v>116</v>
+      </c>
+      <c r="L51" t="s">
+        <v>195</v>
+      </c>
+      <c r="M51" t="s">
+        <v>177</v>
+      </c>
+      <c r="N51" s="56">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="52" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G52" t="s">
+        <v>196</v>
+      </c>
+      <c r="H52" s="54" t="s">
+        <v>179</v>
+      </c>
+      <c r="I52">
+        <v>5</v>
+      </c>
+      <c r="J52">
+        <v>70</v>
+      </c>
+      <c r="K52" t="s">
+        <v>117</v>
+      </c>
+      <c r="L52" t="s">
+        <v>195</v>
+      </c>
+      <c r="M52" t="s">
+        <v>177</v>
+      </c>
+      <c r="N52" s="56">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="53" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G53" t="s">
+        <v>196</v>
+      </c>
+      <c r="H53" s="54" t="s">
+        <v>179</v>
+      </c>
+      <c r="I53">
+        <v>3</v>
+      </c>
+      <c r="J53">
+        <v>92</v>
+      </c>
+      <c r="K53" t="s">
+        <v>117</v>
+      </c>
+      <c r="L53" t="s">
+        <v>194</v>
+      </c>
+      <c r="M53" t="s">
+        <v>177</v>
+      </c>
+      <c r="N53" s="56">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="54" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G54" t="s">
+        <v>196</v>
+      </c>
+      <c r="H54" s="54" t="s">
+        <v>179</v>
+      </c>
+      <c r="I54">
+        <v>5</v>
+      </c>
+      <c r="J54">
+        <v>4</v>
+      </c>
+      <c r="K54" t="s">
+        <v>118</v>
+      </c>
+      <c r="L54" t="s">
+        <v>195</v>
+      </c>
+      <c r="M54" t="s">
+        <v>177</v>
+      </c>
+      <c r="N54" s="56">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="55" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G55" t="s">
+        <v>196</v>
+      </c>
+      <c r="H55" s="54" t="s">
+        <v>179</v>
+      </c>
+      <c r="I55">
+        <v>5</v>
+      </c>
+      <c r="J55">
+        <v>21</v>
+      </c>
+      <c r="K55" t="s">
+        <v>118</v>
+      </c>
+      <c r="L55" t="s">
+        <v>194</v>
+      </c>
+      <c r="M55" t="s">
+        <v>177</v>
+      </c>
+      <c r="N55" s="56">
+        <v>0.86660000000000004</v>
+      </c>
+    </row>
+    <row r="56" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G56" t="s">
+        <v>196</v>
+      </c>
+      <c r="H56" s="54" t="s">
+        <v>179</v>
+      </c>
+      <c r="I56">
+        <v>3</v>
+      </c>
+      <c r="J56">
+        <v>148</v>
+      </c>
+      <c r="K56" t="s">
+        <v>115</v>
+      </c>
+      <c r="L56" t="s">
+        <v>194</v>
+      </c>
+      <c r="M56" t="s">
+        <v>177</v>
+      </c>
+      <c r="N56" s="56">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="57" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G57" t="s">
+        <v>196</v>
+      </c>
+      <c r="H57" s="54" t="s">
+        <v>179</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+      <c r="J57">
+        <v>115</v>
+      </c>
+      <c r="K57" t="s">
+        <v>115</v>
+      </c>
+      <c r="L57" t="s">
+        <v>195</v>
+      </c>
+      <c r="M57" t="s">
+        <v>177</v>
+      </c>
+      <c r="N57" s="56">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="58" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G58" t="s">
+        <v>196</v>
+      </c>
+      <c r="H58" s="54" t="s">
+        <v>179</v>
+      </c>
+      <c r="I58">
+        <v>2</v>
+      </c>
+      <c r="J58">
+        <v>165</v>
+      </c>
+      <c r="K58" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="L58" t="s">
+        <v>195</v>
+      </c>
+      <c r="M58" t="s">
+        <v>177</v>
+      </c>
+      <c r="N58" s="56">
+        <v>0.154</v>
+      </c>
+    </row>
+    <row r="60" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G60" t="s">
+        <v>197</v>
+      </c>
+      <c r="H60" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I60">
+        <v>3</v>
+      </c>
+      <c r="J60">
+        <v>96</v>
+      </c>
+      <c r="K60" t="s">
+        <v>117</v>
+      </c>
+      <c r="L60" t="s">
+        <v>194</v>
+      </c>
+      <c r="M60" t="s">
+        <v>143</v>
+      </c>
+      <c r="N60" s="56">
+        <v>0.53300000000000003</v>
+      </c>
+    </row>
+    <row r="61" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G61" t="s">
+        <v>197</v>
+      </c>
+      <c r="H61" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I61">
+        <v>3</v>
+      </c>
+      <c r="J61">
+        <v>22</v>
+      </c>
+      <c r="K61" t="s">
+        <v>118</v>
+      </c>
+      <c r="L61" t="s">
+        <v>194</v>
+      </c>
+      <c r="M61" t="s">
+        <v>143</v>
+      </c>
+      <c r="N61" s="56">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="62" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G62" t="s">
+        <v>197</v>
+      </c>
+      <c r="H62" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I62">
+        <v>5</v>
+      </c>
+      <c r="J62">
+        <v>65</v>
+      </c>
+      <c r="K62" t="s">
+        <v>117</v>
+      </c>
+      <c r="L62" t="s">
+        <v>195</v>
+      </c>
+      <c r="M62" t="s">
+        <v>177</v>
+      </c>
+      <c r="N62" s="56">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="63" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G63" t="s">
+        <v>197</v>
+      </c>
+      <c r="H63" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I63">
+        <v>5</v>
+      </c>
+      <c r="J63">
+        <v>96</v>
+      </c>
+      <c r="K63" t="s">
+        <v>117</v>
+      </c>
+      <c r="L63" t="s">
+        <v>194</v>
+      </c>
+      <c r="M63" t="s">
+        <v>177</v>
+      </c>
+      <c r="N63" s="56">
+        <v>0.53300000000000003</v>
+      </c>
+    </row>
+    <row r="64" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G64" t="s">
+        <v>197</v>
+      </c>
+      <c r="H64" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I64">
+        <v>5</v>
+      </c>
+      <c r="J64">
+        <v>48</v>
+      </c>
+      <c r="K64" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="L64" t="s">
+        <v>195</v>
+      </c>
+      <c r="M64" t="s">
+        <v>177</v>
+      </c>
+      <c r="N64" s="56">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="65" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G65" t="s">
+        <v>197</v>
+      </c>
+      <c r="H65" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I65">
+        <v>5</v>
+      </c>
+      <c r="J65">
+        <v>22</v>
+      </c>
+      <c r="K65" t="s">
+        <v>118</v>
+      </c>
+      <c r="L65" t="s">
+        <v>194</v>
+      </c>
+      <c r="M65" t="s">
+        <v>177</v>
+      </c>
+      <c r="N65" s="56">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="66" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G66" t="s">
+        <v>197</v>
+      </c>
+      <c r="H66" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I66">
+        <v>2</v>
+      </c>
+      <c r="J66">
+        <v>117</v>
+      </c>
+      <c r="K66" t="s">
+        <v>115</v>
+      </c>
+      <c r="L66" t="s">
+        <v>195</v>
+      </c>
+      <c r="M66" t="s">
+        <v>177</v>
+      </c>
+      <c r="N66" s="56">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="67" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G67" t="s">
+        <v>197</v>
+      </c>
+      <c r="H67" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I67">
+        <v>1</v>
+      </c>
+      <c r="J67">
+        <v>116</v>
+      </c>
+      <c r="K67" t="s">
+        <v>115</v>
+      </c>
+      <c r="L67" t="s">
+        <v>195</v>
+      </c>
+      <c r="M67" t="s">
+        <v>177</v>
+      </c>
+      <c r="N67" s="56">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="68" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G68" t="s">
+        <v>197</v>
+      </c>
+      <c r="H68" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="I68">
+        <v>4</v>
+      </c>
+      <c r="J68">
+        <v>150</v>
+      </c>
+      <c r="K68" t="s">
+        <v>115</v>
+      </c>
+      <c r="L68" t="s">
+        <v>194</v>
+      </c>
+      <c r="M68" t="s">
+        <v>177</v>
+      </c>
+      <c r="N68" s="56">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="69" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G69" t="s">
+        <v>197</v>
+      </c>
+      <c r="H69" s="54" t="s">
+        <v>179</v>
+      </c>
+      <c r="I69">
+        <v>5</v>
+      </c>
+      <c r="J69">
+        <v>33</v>
+      </c>
+      <c r="K69" t="s">
+        <v>118</v>
+      </c>
+      <c r="L69" t="s">
+        <v>194</v>
+      </c>
+      <c r="M69" t="s">
+        <v>177</v>
+      </c>
+      <c r="N69" s="56">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="70" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G70" t="s">
+        <v>197</v>
+      </c>
+      <c r="H70" s="54" t="s">
+        <v>179</v>
+      </c>
+      <c r="I70">
+        <v>1</v>
+      </c>
+      <c r="J70">
+        <v>43</v>
+      </c>
+      <c r="K70" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="L70" t="s">
+        <v>195</v>
+      </c>
+      <c r="M70" t="s">
+        <v>177</v>
+      </c>
+      <c r="N70" s="56">
+        <v>6.6600000000000006E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G71" t="s">
+        <v>197</v>
+      </c>
+      <c r="H71" s="54" t="s">
+        <v>179</v>
+      </c>
+      <c r="I71">
+        <v>3</v>
+      </c>
+      <c r="J71">
+        <v>116</v>
+      </c>
+      <c r="K71" t="s">
+        <v>115</v>
+      </c>
+      <c r="L71" t="s">
+        <v>195</v>
+      </c>
+      <c r="M71" t="s">
+        <v>177</v>
+      </c>
+      <c r="N71" s="56">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="72" spans="7:14" x14ac:dyDescent="0.2">
+      <c r="G72" t="s">
+        <v>197</v>
+      </c>
+      <c r="H72" s="54" t="s">
+        <v>179</v>
+      </c>
+      <c r="I72">
+        <v>4</v>
+      </c>
+      <c r="J72">
+        <v>159</v>
+      </c>
+      <c r="K72" t="s">
+        <v>116</v>
+      </c>
+      <c r="L72" t="s">
+        <v>195</v>
+      </c>
+      <c r="M72" t="s">
+        <v>177</v>
+      </c>
+      <c r="N72" s="56">
+        <v>0.28570000000000001</v>
+      </c>
+    </row>
+    <row r="1048576" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G1048576" s="53"/>
+      <c r="H1048576" s="54"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G3:N17">
+    <sortCondition ref="M3:M17"/>
+    <sortCondition ref="H3:H17"/>
+    <sortCondition ref="K3:K17"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>